<commit_message>
modifictation titre graphique et position graphique
</commit_message>
<xml_diff>
--- a/data/variables EVOLUTIONS_OJ.xlsx
+++ b/data/variables EVOLUTIONS_OJ.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noack\gitCereq\cereq-dataviz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D1DE4D3-3C1C-40E7-BE1F-F74252AED8DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A753701-F6E3-4EDA-BEE2-A10F5A3385DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19320" yWindow="360" windowWidth="19440" windowHeight="15000" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -113,9 +113,6 @@
     <t>competence_ok</t>
   </si>
   <si>
-    <t xml:space="preserve">Proportion de jeunes dans une autre situation (formation, inactivité, reprise d'études) </t>
-  </si>
-  <si>
     <t xml:space="preserve">Proportion de jeunes en emploi à durée indéterminée </t>
   </si>
   <si>
@@ -135,6 +132,9 @@
   </si>
   <si>
     <t>Trois années après la fin de formation initiale</t>
+  </si>
+  <si>
+    <t>Proportion de jeunes à temps partiel</t>
   </si>
 </sst>
 </file>
@@ -555,7 +555,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -592,7 +592,7 @@
         <v>21</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -617,7 +617,7 @@
         <v>23</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -628,10 +628,10 @@
         <v>6</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -642,7 +642,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -653,10 +653,10 @@
         <v>7</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -748,7 +748,7 @@
         <v>24</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -768,6 +768,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e8254419-5e3e-4d09-9ab1-694bd035361a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a3559f96-a391-4298-a476-5fa029e2109e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000DCE2AD71575ED409F6CD8D87660A7B5" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e7a409e0b47e02996c47cd99ab55c69c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a3559f96-a391-4298-a476-5fa029e2109e" xmlns:ns3="e8254419-5e3e-4d09-9ab1-694bd035361a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ec4d4004c5339e4d0b1f4fd079361e4" ns2:_="" ns3:_="">
     <xsd:import namespace="a3559f96-a391-4298-a476-5fa029e2109e"/>
@@ -990,17 +1001,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e8254419-5e3e-4d09-9ab1-694bd035361a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a3559f96-a391-4298-a476-5fa029e2109e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1011,6 +1011,17 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
+    <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DD558F8-9C61-4625-9943-A9AFF41A0CEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1029,17 +1040,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
-    <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
modif du i de tx d'emploi
</commit_message>
<xml_diff>
--- a/data/variables EVOLUTIONS_OJ.xlsx
+++ b/data/variables EVOLUTIONS_OJ.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noack\gitCereq\cereq-dataviz\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A753701-F6E3-4EDA-BEE2-A10F5A3385DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B516FEB9-04B7-43AE-8E93-07A3E8373F87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{0FDA0247-04C8-41EE-A704-5099EBC3E1E6}"/>
   </bookViews>
@@ -131,17 +131,17 @@
     <t>Niveau de salaire ou traitement mensuel net primes incluses médian. Le revenu médian est la valeur telle que la moitié des jeunes de la population considérée gagne plus, l'autre moitié gagne  moins.</t>
   </si>
   <si>
-    <t>Trois années après la fin de formation initiale</t>
-  </si>
-  <si>
     <t>Proportion de jeunes à temps partiel</t>
+  </si>
+  <si>
+    <t>Le taux d'emploi correspond à la part des individus en emploi parmi la population totale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -187,6 +187,12 @@
       <name val="Courier"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -237,6 +243,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -555,7 +564,7 @@
   <dimension ref="A1:D20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -591,8 +600,8 @@
       <c r="C2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>31</v>
+      <c r="D2" s="11" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -642,7 +651,7 @@
         <v>17</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
@@ -768,17 +777,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="e8254419-5e3e-4d09-9ab1-694bd035361a" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a3559f96-a391-4298-a476-5fa029e2109e">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000DCE2AD71575ED409F6CD8D87660A7B5" ma:contentTypeVersion="13" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="e7a409e0b47e02996c47cd99ab55c69c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a3559f96-a391-4298-a476-5fa029e2109e" xmlns:ns3="e8254419-5e3e-4d09-9ab1-694bd035361a" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6ec4d4004c5339e4d0b1f4fd079361e4" ns2:_="" ns3:_="">
     <xsd:import namespace="a3559f96-a391-4298-a476-5fa029e2109e"/>
@@ -1001,6 +999,17 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="e8254419-5e3e-4d09-9ab1-694bd035361a" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="a3559f96-a391-4298-a476-5fa029e2109e">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1011,17 +1020,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
-    <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9DD558F8-9C61-4625-9943-A9AFF41A0CEC}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1040,6 +1038,17 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1C982F7B-9F64-4BB5-A7EE-B02A98A3CE38}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e8254419-5e3e-4d09-9ab1-694bd035361a"/>
+    <ds:schemaRef ds:uri="a3559f96-a391-4298-a476-5fa029e2109e"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6ED99F3F-669F-4292-BE5F-AA397ACBBD82}">
   <ds:schemaRefs>

</xml_diff>